<commit_message>
Started basic hyperparameter optimization, continued editing pca_analysis instructions, and added some new document modification tooling for the new pos / neg data currently coming through.
</commit_message>
<xml_diff>
--- a/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
+++ b/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>121</v>
+        <v>26</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>136</v>
+        <v>16</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -980,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="n">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1118,7 +1118,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="n">
-        <v>168</v>
+        <v>72</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>176</v>
+        <v>59</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="n">
-        <v>177</v>
+        <v>60</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="n">
-        <v>169</v>
+        <v>58</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1233,7 +1233,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="n">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="n">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>15</v>
       </c>
       <c r="C37" t="n">
-        <v>376</v>
+        <v>81</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="n">
-        <v>304</v>
+        <v>97</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1325,7 +1325,7 @@
         <v>17</v>
       </c>
       <c r="C39" t="n">
-        <v>248</v>
+        <v>19</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1348,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="C40" t="n">
-        <v>249</v>
+        <v>31</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="n">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1394,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="C42" t="n">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Reverted default group numbers and metadata so they are consistent with the other default paths and data.
</commit_message>
<xml_diff>
--- a/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
+++ b/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>62</v>
+        <v>231</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>65</v>
+        <v>287</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -980,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="n">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1118,7 +1118,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>179</v>
+        <v>85</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="n">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="n">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="n">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1233,7 +1233,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="n">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="n">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>15</v>
       </c>
       <c r="C37" t="n">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="n">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1325,7 +1325,7 @@
         <v>17</v>
       </c>
       <c r="C39" t="n">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1348,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="C40" t="n">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="n">
-        <v>120</v>
+        <v>73</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1394,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="C42" t="n">
-        <v>181</v>
+        <v>66</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fixed description being written directly to report in list format and fixed incorrect indexing of DataFrame.  Also removed last uses of metadata and group number files and made parallel changes to update the older main.py.
</commit_message>
<xml_diff>
--- a/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
+++ b/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>125</v>
+        <v>39</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>231</v>
+        <v>70</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>159</v>
+        <v>53</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>287</v>
+        <v>72</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -980,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1118,7 +1118,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="n">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="n">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="n">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1233,7 +1233,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="n">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>15</v>
       </c>
       <c r="C37" t="n">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="n">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1325,7 +1325,7 @@
         <v>17</v>
       </c>
       <c r="C39" t="n">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1348,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="C40" t="n">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="n">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1394,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="C42" t="n">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fixed hard-coded values overriding strings grabbed from text fields in user interface in main_test.  Also improved title of PCA report.
</commit_message>
<xml_diff>
--- a/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
+++ b/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>59</v>
+        <v>175</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>99</v>
+        <v>231</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>60</v>
+        <v>287</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -980,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="n">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1118,7 +1118,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="n">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="n">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="n">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1233,7 +1233,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="n">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>15</v>
       </c>
       <c r="C37" t="n">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="n">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1325,7 +1325,7 @@
         <v>17</v>
       </c>
       <c r="C39" t="n">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1348,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="C40" t="n">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="n">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1394,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="C42" t="n">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fixed issue with sample numbers 001-006 causing false positive data columns to be included in PCA plots.
</commit_message>
<xml_diff>
--- a/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
+++ b/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>175</v>
+        <v>19</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>231</v>
+        <v>60</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>287</v>
+        <v>138</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -980,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1118,7 +1118,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="n">
-        <v>99</v>
+        <v>175</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1233,7 +1233,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="n">
-        <v>110</v>
+        <v>231</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="n">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>15</v>
       </c>
       <c r="C37" t="n">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="n">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1325,7 +1325,7 @@
         <v>17</v>
       </c>
       <c r="C39" t="n">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1348,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="C40" t="n">
-        <v>55</v>
+        <v>159</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1394,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="C42" t="n">
-        <v>137</v>
+        <v>1</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Updated all reports with example data using the catalog system.
</commit_message>
<xml_diff>
--- a/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
+++ b/SIMS_PCA/SIMS_PCA/output_sample/LoadingPC1.xlsx
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>138</v>
+        <v>60</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -980,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>125</v>
+        <v>28</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="n">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="n">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="n">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="n">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1233,7 +1233,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="n">
-        <v>231</v>
+        <v>91</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>15</v>
       </c>
       <c r="C37" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="n">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1325,7 +1325,7 @@
         <v>17</v>
       </c>
       <c r="C39" t="n">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="n">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1394,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>

</xml_diff>